<commit_message>
Introduce padded batches and masking to allow for batches with size different from 1, even if input sequences have different lengths. Introduce batch normalization thanks to the new batch size > 1. Introduce several datasets and refactor the files to always have the same format: musicxml for scores and csv for chords. All chords analysis now start at offset 0, regardless of pickup measures. This has been adapted since is the standard for music21 when it reads scores. Refactor the code regarding chord_root_finding and segment_chord_labels. Remove the 'sonata' and 'transposed' keywords from the tfrecords. Add a playground.py file to quickly analyse the dataset. Correct some errors in the BPS-FH dataset.
</commit_message>
<xml_diff>
--- a/data/BPS_FH_Dataset/02/chords.xlsx
+++ b/data/BPS_FH_Dataset/02/chords.xlsx
@@ -415,8 +415,8 @@
   </sheetPr>
   <dimension ref="A1:O459"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A304" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J324" activeCellId="0" sqref="J324"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,7 +427,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="B1" s="1" t="n">
         <v>4</v>
@@ -4788,7 +4788,7 @@
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="n">
-        <v>544</v>
+        <v>554</v>
       </c>
       <c r="B187" s="1" t="n">
         <v>558</v>

</xml_diff>